<commit_message>
added support for onchain inferred cases
</commit_message>
<xml_diff>
--- a/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
+++ b/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1078"/>
+  <dimension ref="A1:E1079"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20923,6 +20923,25 @@
         <v>263200000</v>
       </c>
     </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>2023-11-29T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1079" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1079" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1079" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1079" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
simple change in comments
</commit_message>
<xml_diff>
--- a/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
+++ b/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1079"/>
+  <dimension ref="A1:E1100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20942,6 +20942,405 @@
         <v>263200000</v>
       </c>
     </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>2023-11-30T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1080" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1080" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1080" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1080" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>2023-12-01T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1081" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1081" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1081" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1081" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>2023-12-02T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1082" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1082" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1082" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1082" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>2023-12-03T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1083" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1083" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1083" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1083" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>2023-12-04T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1084" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1084" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1084" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1084" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>2023-12-05T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1085" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1085" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1085" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1085" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>2023-12-06T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1086" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1086" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1086" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1086" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>2023-12-07T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1087" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1087" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1087" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1087" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>2023-12-08T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1088" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1088" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1088" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1088" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>2023-12-09T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1089" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1089" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1089" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1089" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>2023-12-10T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1090" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1090" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1090" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1090" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>2023-12-11T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1091" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1091" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1091" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1091" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>2023-12-12T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1092" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1092" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1092" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1092" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>2023-12-13T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1093" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1093" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1093" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1093" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>2023-12-14T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1094" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1094" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1094" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1094" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>2023-12-15T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1095" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1095" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1095" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1095" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>2023-12-16T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1096" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1096" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1096" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1096" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>2023-12-17T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1097" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1097" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1097" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1097" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>2023-12-18T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1098" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1098" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1098" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1098" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>2023-12-19T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1099" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1099" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1099" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1099" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>2023-12-20T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1100" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1100" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1100" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1100" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
minor fixes with tokenUnlocks
</commit_message>
<xml_diff>
--- a/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
+++ b/XUnlocksCrawler/output/tu/chartData_LDO_lido-dao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1161"/>
+  <dimension ref="A1:E1169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22500,6 +22500,158 @@
         <v>263200000</v>
       </c>
     </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>2024-02-20T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1162" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1162" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1162" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1162" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>2024-02-21T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1163" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1163" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1163" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1163" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>2024-02-22T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1164" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1164" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1164" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1164" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>2024-02-23T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1165" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1165" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1165" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1165" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>2024-02-24T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1166" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1166" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1166" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1166" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>2024-02-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1167" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1167" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1167" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1167" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>2024-02-26T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1168" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1168" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1168" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1168" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>2024-02-27T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B1169" t="n">
+        <v>353806241</v>
+      </c>
+      <c r="C1169" t="n">
+        <v>60400000</v>
+      </c>
+      <c r="D1169" t="n">
+        <v>340000000</v>
+      </c>
+      <c r="E1169" t="n">
+        <v>263200000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>